<commit_message>
Add utilities module, add a form to the analysis file, clean up both analysis and players leaving files
</commit_message>
<xml_diff>
--- a/data/datasets/roster_fresno_state.xlsx
+++ b/data/datasets/roster_fresno_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96639D2F-D3B9-4D6E-A6D2-B4E0A66B3995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49A430A-0E45-4003-A3A3-6E633180AC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="266">
   <si>
     <t>first_name</t>
   </si>
@@ -871,10 +871,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -903,8 +903,8 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="team"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="archetype"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="dev_trait"/>
-    <tableColumn id="12" xr3:uid="{F985EAEC-8A5C-4803-BB3E-555C51872002}" name="overall_start" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="overall_end" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{F985EAEC-8A5C-4803-BB3E-555C51872002}" name="overall_start" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="overall_end" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1200,7 +1200,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+      <selection activeCell="J105" sqref="J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,7 +1387,9 @@
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K5" s="1">
         <v>78</v>
       </c>
@@ -1421,7 +1423,9 @@
       <c r="I6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="K6" s="1">
         <v>78</v>
       </c>
@@ -1489,7 +1493,9 @@
       <c r="I8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="K8" s="1">
         <v>74</v>
       </c>
@@ -1693,7 +1699,9 @@
       <c r="I14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K14" s="1">
         <v>80</v>
       </c>
@@ -1727,7 +1735,9 @@
       <c r="I15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K15" s="1">
         <v>80</v>
       </c>
@@ -1761,7 +1771,9 @@
       <c r="I16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="K16" s="1">
         <v>78</v>
       </c>
@@ -1795,7 +1807,9 @@
       <c r="I17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K17" s="1">
         <v>75</v>
       </c>
@@ -2033,7 +2047,9 @@
       <c r="I24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="K24" s="1">
         <v>75</v>
       </c>
@@ -2067,7 +2083,9 @@
       <c r="I25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K25" s="1">
         <v>74</v>
       </c>
@@ -2101,7 +2119,9 @@
       <c r="I26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K26" s="1">
         <v>73</v>
       </c>
@@ -2169,7 +2189,9 @@
       <c r="I28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K28" s="1">
         <v>70</v>
       </c>
@@ -2203,7 +2225,9 @@
       <c r="I29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K29" s="1">
         <v>65</v>
       </c>
@@ -2373,7 +2397,9 @@
       <c r="I34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="K34" s="1">
         <v>78</v>
       </c>
@@ -2441,6 +2467,9 @@
       <c r="I36" t="s">
         <v>35</v>
       </c>
+      <c r="J36" t="s">
+        <v>17</v>
+      </c>
       <c r="K36">
         <v>73</v>
       </c>
@@ -2677,7 +2706,9 @@
       <c r="I43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K43" s="1">
         <v>76</v>
       </c>
@@ -2779,7 +2810,9 @@
       <c r="I46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J46" s="1"/>
+      <c r="J46" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K46" s="1">
         <v>74</v>
       </c>
@@ -2949,7 +2982,9 @@
       <c r="I51" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J51" s="1"/>
+      <c r="J51" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K51" s="1">
         <v>74</v>
       </c>
@@ -3085,7 +3120,9 @@
       <c r="I55" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J55" s="1"/>
+      <c r="J55" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K55" s="1">
         <v>76</v>
       </c>
@@ -3221,7 +3258,9 @@
       <c r="I59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J59" s="1"/>
+      <c r="J59" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K59" s="1">
         <v>69</v>
       </c>
@@ -3357,7 +3396,9 @@
       <c r="I63" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J63" s="1"/>
+      <c r="J63" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K63" s="1">
         <v>76</v>
       </c>
@@ -3527,7 +3568,9 @@
       <c r="I68" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J68" s="1"/>
+      <c r="J68" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K68" s="1">
         <v>71</v>
       </c>
@@ -3595,7 +3638,9 @@
       <c r="I70" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J70" s="1"/>
+      <c r="J70" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K70" s="1">
         <v>76</v>
       </c>
@@ -3629,7 +3674,9 @@
       <c r="I71" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J71" s="1"/>
+      <c r="J71" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K71" s="1">
         <v>73</v>
       </c>
@@ -3833,7 +3880,9 @@
       <c r="I77" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J77" s="1"/>
+      <c r="J77" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K77" s="1">
         <v>77</v>
       </c>
@@ -4003,7 +4052,9 @@
       <c r="I82" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J82" s="1"/>
+      <c r="J82" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K82" s="1">
         <v>67</v>
       </c>
@@ -4241,7 +4292,9 @@
       <c r="I89" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J89" s="1"/>
+      <c r="J89" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="K89" s="1">
         <v>76</v>
       </c>
@@ -4275,7 +4328,9 @@
       <c r="I90" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J90" s="1"/>
+      <c r="J90" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K90" s="1">
         <v>74</v>
       </c>
@@ -4343,7 +4398,9 @@
       <c r="I92" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J92" s="1"/>
+      <c r="J92" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K92" s="1">
         <v>68</v>
       </c>
@@ -4513,7 +4570,9 @@
       <c r="I97" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J97" s="1"/>
+      <c r="J97" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K97" s="1">
         <v>74</v>
       </c>
@@ -4649,7 +4708,9 @@
       <c r="I101" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J101" s="1"/>
+      <c r="J101" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K101" s="1">
         <v>67</v>
       </c>
@@ -4717,7 +4778,9 @@
       <c r="I103" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J103" s="1"/>
+      <c r="J103" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K103" s="1">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Fix small errors in 2029 rosters
</commit_message>
<xml_diff>
--- a/data/datasets/roster_fresno_state.xlsx
+++ b/data/datasets/roster_fresno_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927B7B63-6463-4D48-AD76-4A1F8F296F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17162CB-3DC3-4088-B4BB-3299C7C76D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="231">
   <si>
     <t>first_name</t>
   </si>
@@ -779,8 +779,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Frame2" displayName="Frame2" ref="A1:L86" totalsRowShown="0">
-  <autoFilter ref="A1:L86" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Frame2" displayName="Frame2" ref="A1:L85" totalsRowShown="0">
+  <autoFilter ref="A1:L85" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="first_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="last_name"/>
@@ -1086,11 +1086,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2059,16 +2057,16 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="A26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="1" t="b">
+      <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -2083,66 +2081,66 @@
       <c r="H26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" t="s">
         <v>33</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26" s="1">
-        <v>80</v>
-      </c>
-      <c r="L26" s="1">
-        <v>80</v>
+      <c r="J26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26">
+        <v>73</v>
+      </c>
+      <c r="L26">
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I27" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27">
-        <v>73</v>
-      </c>
-      <c r="L27">
-        <v>73</v>
+        <v>26</v>
+      </c>
+      <c r="K27" s="1">
+        <v>92</v>
+      </c>
+      <c r="L27" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C28" t="s">
-        <v>19</v>
+      <c r="A28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -2159,28 +2157,28 @@
       <c r="H28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J28" t="s">
-        <v>26</v>
+      <c r="J28" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="K28" s="1">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="L28" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>25</v>
+      <c r="A29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -2197,37 +2195,37 @@
       <c r="H29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>14</v>
+      <c r="I29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" t="s">
+        <v>17</v>
       </c>
       <c r="K29" s="1">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L29" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" t="s">
-        <v>126</v>
-      </c>
-      <c r="C30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" t="b">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>36</v>
@@ -2235,28 +2233,28 @@
       <c r="H30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I30" t="s">
-        <v>41</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="I30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="1">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="L30" s="1">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D31" s="1" t="b">
         <v>1</v>
@@ -2274,30 +2272,30 @@
         <v>12</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K31" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L31" s="1">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>39</v>
@@ -2315,33 +2313,33 @@
         <v>41</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="K32" s="1">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="L32" s="1">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>36</v>
@@ -2353,24 +2351,24 @@
         <v>41</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="K33" s="1">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="L33" s="1">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D34" s="1" t="b">
         <v>1</v>
@@ -2388,24 +2386,24 @@
         <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K34" s="1">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="L34" s="1">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -2426,36 +2424,36 @@
         <v>12</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K35" s="1">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="L35" s="1">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>36</v>
@@ -2464,36 +2462,36 @@
         <v>12</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K36" s="1">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="L36" s="1">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D37" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>36</v>
@@ -2502,30 +2500,30 @@
         <v>12</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K37" s="1">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="L37" s="1">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D38" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>44</v>
@@ -2540,36 +2538,36 @@
         <v>12</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="K38" s="1">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="L38" s="1">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>36</v>
@@ -2581,33 +2579,33 @@
         <v>37</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K39" s="1">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="L39" s="1">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D40" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>36</v>
@@ -2616,27 +2614,27 @@
         <v>12</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="K40" s="1">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L40" s="1">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D41" s="1" t="b">
         <v>1</v>
@@ -2657,27 +2655,27 @@
         <v>37</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K41" s="1">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="L41" s="1">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>165</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D42" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>49</v>
@@ -2695,100 +2693,100 @@
         <v>37</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="K42" s="1">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L42" s="1">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>99</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>167</v>
+        <v>97</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D43" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K43" s="1">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="L43" s="1">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="K44" s="1">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="L44" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D45" s="1" t="b">
         <v>1</v>
@@ -2812,24 +2810,24 @@
         <v>17</v>
       </c>
       <c r="K45" s="1">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L45" s="1">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D46" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>50</v>
@@ -2847,21 +2845,21 @@
         <v>55</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="K46" s="1">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L46" s="1">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>25</v>
@@ -2870,7 +2868,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>51</v>
@@ -2885,30 +2883,30 @@
         <v>54</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K47" s="1">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="L47" s="1">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>51</v>
@@ -2923,24 +2921,24 @@
         <v>55</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K48" s="1">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="L48" s="1">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D49" s="1" t="b">
         <v>1</v>
@@ -2958,30 +2956,30 @@
         <v>53</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K49" s="1">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="L49" s="1">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>72</v>
+        <v>176</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D50" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>58</v>
@@ -3002,30 +3000,30 @@
         <v>14</v>
       </c>
       <c r="K50" s="1">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="L50" s="1">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D51" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>52</v>
@@ -3037,33 +3035,33 @@
         <v>55</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K51" s="1">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="L51" s="1">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D52" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>52</v>
@@ -3072,24 +3070,24 @@
         <v>53</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="K52" s="1">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="L52" s="1">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>149</v>
+        <v>95</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>25</v>
@@ -3110,30 +3108,30 @@
         <v>53</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="K53" s="1">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L53" s="1">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D54" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>60</v>
@@ -3148,51 +3146,51 @@
         <v>53</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K54" s="1">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="L54" s="1">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D55" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>53</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="K55" s="1">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L55" s="1">
         <v>80</v>
@@ -3200,10 +3198,10 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>18</v>
@@ -3212,13 +3210,13 @@
         <v>0</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>53</v>
@@ -3230,24 +3228,24 @@
         <v>17</v>
       </c>
       <c r="K56" s="1">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="L56" s="1">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D57" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>65</v>
@@ -3265,33 +3263,33 @@
         <v>54</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K57" s="1">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="L57" s="1">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D58" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>67</v>
@@ -3300,36 +3298,36 @@
         <v>53</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K58" s="1">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="L58" s="1">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>188</v>
+        <v>56</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D59" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>67</v>
@@ -3338,27 +3336,27 @@
         <v>53</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K59" s="1">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="L59" s="1">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D60" s="1" t="b">
         <v>1</v>
@@ -3376,30 +3374,30 @@
         <v>53</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="K60" s="1">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L60" s="1">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D61" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>70</v>
@@ -3414,36 +3412,36 @@
         <v>53</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K61" s="1">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="L61" s="1">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>192</v>
+        <v>91</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D62" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>67</v>
@@ -3452,36 +3450,36 @@
         <v>53</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K62" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L62" s="1">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>195</v>
+        <v>48</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D63" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>67</v>
@@ -3490,27 +3488,27 @@
         <v>53</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="K63" s="1">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="L63" s="1">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D64" s="1" t="b">
         <v>1</v>
@@ -3531,24 +3529,24 @@
         <v>69</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="K64" s="1">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L64" s="1">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D65" s="1" t="b">
         <v>1</v>
@@ -3566,30 +3564,30 @@
         <v>53</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K65" s="1">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="L65" s="1">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D66" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>71</v>
@@ -3604,103 +3602,103 @@
         <v>53</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K66" s="1">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="L66" s="1">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>199</v>
+        <v>45</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D67" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>53</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K67" s="1">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="L67" s="1">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D68" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>53</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K68" s="1">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="L68" s="1">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D69" s="1" t="b">
         <v>1</v>
@@ -3718,13 +3716,13 @@
         <v>53</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="K69" s="1">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L69" s="1">
         <v>90</v>
@@ -3732,10 +3730,10 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>25</v>
@@ -3756,27 +3754,27 @@
         <v>53</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K70" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L70" s="1">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D71" s="1" t="b">
         <v>1</v>
@@ -3797,24 +3795,24 @@
         <v>77</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K71" s="1">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L71" s="1">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D72" s="1" t="b">
         <v>1</v>
@@ -3832,68 +3830,68 @@
         <v>53</v>
       </c>
       <c r="I72" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K72" s="1">
         <v>83</v>
       </c>
-      <c r="J72" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K72" s="1">
-        <v>91</v>
-      </c>
       <c r="L72" s="1">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>209</v>
+        <v>139</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D73" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="K73" s="1">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L73" s="1">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>74</v>
@@ -3908,24 +3906,24 @@
         <v>53</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>46</v>
       </c>
       <c r="K74" s="1">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="L74" s="1">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>18</v>
@@ -3949,21 +3947,21 @@
         <v>76</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="K75" s="1">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L75" s="1">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>85</v>
+        <v>214</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>18</v>
@@ -3987,33 +3985,33 @@
         <v>76</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K76" s="1">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L76" s="1">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D77" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>75</v>
@@ -4022,27 +4020,27 @@
         <v>53</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K77" s="1">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="L77" s="1">
-        <v>68</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D78" s="1" t="b">
         <v>1</v>
@@ -4060,30 +4058,30 @@
         <v>53</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K78" s="1">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="L78" s="1">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D79" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>81</v>
@@ -4101,30 +4099,30 @@
         <v>84</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="K79" s="1">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="L79" s="1">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D80" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>82</v>
@@ -4139,24 +4137,24 @@
         <v>84</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="K80" s="1">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L80" s="1">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D81" s="1" t="b">
         <v>1</v>
@@ -4174,30 +4172,30 @@
         <v>53</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K81" s="1">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L81" s="1">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>43</v>
+        <v>224</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D82" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>86</v>
@@ -4212,65 +4210,65 @@
         <v>53</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K82" s="1">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="L82" s="1">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>224</v>
+        <v>100</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D83" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K83" s="1">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="L83" s="1">
-        <v>67</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>100</v>
+        <v>227</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D84" s="1" t="b">
         <v>0</v>
@@ -4291,30 +4289,30 @@
         <v>38</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K84" s="1">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L84" s="1">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D85" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>87</v>
@@ -4332,49 +4330,25 @@
         <v>14</v>
       </c>
       <c r="K85" s="1">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="L85" s="1">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D86" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K86" s="1">
-        <v>73</v>
-      </c>
-      <c r="L86" s="1">
         <v>71</v>
       </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
@@ -4461,10 +4435,6 @@
       <c r="L95" s="1"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
@@ -4478,7 +4448,6 @@
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
@@ -4489,6 +4458,10 @@
       <c r="L97" s="1"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
@@ -4502,6 +4475,7 @@
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
@@ -4609,34 +4583,6 @@
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
-      <c r="J107" s="1"/>
-      <c r="K107" s="1"/>
-      <c r="L107" s="1"/>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
-      <c r="K108" s="1"/>
-      <c r="L108" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update rosters with 2029 overall_end values
</commit_message>
<xml_diff>
--- a/data/datasets/roster_fresno_state.xlsx
+++ b/data/datasets/roster_fresno_state.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17162CB-3DC3-4088-B4BB-3299C7C76D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0706A2-4CA3-4458-AB6C-AE20737446FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2029" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -1088,7 +1088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1255,7 +1257,7 @@
         <v>78</v>
       </c>
       <c r="L4" s="1">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1331,7 +1333,7 @@
         <v>90</v>
       </c>
       <c r="L6" s="1">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1369,7 +1371,7 @@
         <v>87</v>
       </c>
       <c r="L7" s="1">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1407,7 +1409,7 @@
         <v>85</v>
       </c>
       <c r="L8" s="1">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1483,7 +1485,7 @@
         <v>80</v>
       </c>
       <c r="L10" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1521,7 +1523,7 @@
         <v>78</v>
       </c>
       <c r="L11" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1597,7 +1599,7 @@
         <v>91</v>
       </c>
       <c r="L13" s="1">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1635,7 +1637,7 @@
         <v>91</v>
       </c>
       <c r="L14" s="1">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1673,7 +1675,7 @@
         <v>87</v>
       </c>
       <c r="L15" s="1">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1711,7 +1713,7 @@
         <v>85</v>
       </c>
       <c r="L16" s="1">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1749,7 +1751,7 @@
         <v>79</v>
       </c>
       <c r="L17" s="1">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1787,7 +1789,7 @@
         <v>76</v>
       </c>
       <c r="L18" s="1">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1825,7 +1827,7 @@
         <v>74</v>
       </c>
       <c r="L19" s="1">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1977,7 +1979,7 @@
         <v>93</v>
       </c>
       <c r="L23" s="1">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2015,7 +2017,7 @@
         <v>89</v>
       </c>
       <c r="L24" s="1">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2053,7 +2055,7 @@
         <v>82</v>
       </c>
       <c r="L25" s="1">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2091,7 +2093,7 @@
         <v>73</v>
       </c>
       <c r="L26">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2129,7 +2131,7 @@
         <v>92</v>
       </c>
       <c r="L27" s="1">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2167,7 +2169,7 @@
         <v>83</v>
       </c>
       <c r="L28" s="1">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -2205,7 +2207,7 @@
         <v>81</v>
       </c>
       <c r="L29" s="1">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -2243,7 +2245,7 @@
         <v>86</v>
       </c>
       <c r="L30" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2281,7 +2283,7 @@
         <v>85</v>
       </c>
       <c r="L31" s="1">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -2357,7 +2359,7 @@
         <v>86</v>
       </c>
       <c r="L33" s="1">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2395,7 +2397,7 @@
         <v>78</v>
       </c>
       <c r="L34" s="1">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2471,7 +2473,7 @@
         <v>90</v>
       </c>
       <c r="L36" s="1">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -2509,7 +2511,7 @@
         <v>83</v>
       </c>
       <c r="L37" s="1">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2585,7 +2587,7 @@
         <v>89</v>
       </c>
       <c r="L39" s="1">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2661,7 +2663,7 @@
         <v>82</v>
       </c>
       <c r="L41" s="1">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -2737,7 +2739,7 @@
         <v>91</v>
       </c>
       <c r="L43" s="1">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -2775,7 +2777,7 @@
         <v>88</v>
       </c>
       <c r="L44" s="1">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2889,7 +2891,7 @@
         <v>88</v>
       </c>
       <c r="L47" s="1">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -2927,7 +2929,7 @@
         <v>86</v>
       </c>
       <c r="L48" s="1">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2965,7 +2967,7 @@
         <v>80</v>
       </c>
       <c r="L49" s="1">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -3041,7 +3043,7 @@
         <v>91</v>
       </c>
       <c r="L51" s="1">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3079,7 +3081,7 @@
         <v>89</v>
       </c>
       <c r="L52" s="1">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3117,7 +3119,7 @@
         <v>86</v>
       </c>
       <c r="L53" s="1">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -3193,7 +3195,7 @@
         <v>89</v>
       </c>
       <c r="L55" s="1">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -3231,7 +3233,7 @@
         <v>76</v>
       </c>
       <c r="L56" s="1">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -3269,7 +3271,7 @@
         <v>73</v>
       </c>
       <c r="L57" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -3307,7 +3309,7 @@
         <v>92</v>
       </c>
       <c r="L58" s="1">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3345,7 +3347,7 @@
         <v>90</v>
       </c>
       <c r="L59" s="1">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -3383,7 +3385,7 @@
         <v>87</v>
       </c>
       <c r="L60" s="1">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -3421,7 +3423,7 @@
         <v>77</v>
       </c>
       <c r="L61" s="1">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -3459,7 +3461,7 @@
         <v>86</v>
       </c>
       <c r="L62" s="1">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
@@ -3535,7 +3537,7 @@
         <v>83</v>
       </c>
       <c r="L64" s="1">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -3573,7 +3575,7 @@
         <v>76</v>
       </c>
       <c r="L65" s="1">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -3611,7 +3613,7 @@
         <v>67</v>
       </c>
       <c r="L66" s="1">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -3649,7 +3651,7 @@
         <v>94</v>
       </c>
       <c r="L67" s="1">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -3687,7 +3689,7 @@
         <v>92</v>
       </c>
       <c r="L68" s="1">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -3725,7 +3727,7 @@
         <v>91</v>
       </c>
       <c r="L69" s="1">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -3763,7 +3765,7 @@
         <v>91</v>
       </c>
       <c r="L70" s="1">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -3801,7 +3803,7 @@
         <v>86</v>
       </c>
       <c r="L71" s="1">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -3839,7 +3841,7 @@
         <v>83</v>
       </c>
       <c r="L72" s="1">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -3856,16 +3858,16 @@
         <v>0</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>33</v>
@@ -3877,7 +3879,7 @@
         <v>80</v>
       </c>
       <c r="L73" s="1">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -4029,7 +4031,7 @@
         <v>96</v>
       </c>
       <c r="L77" s="1">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -4067,7 +4069,7 @@
         <v>82</v>
       </c>
       <c r="L78" s="1">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -4143,7 +4145,7 @@
         <v>82</v>
       </c>
       <c r="L80" s="1">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -4181,7 +4183,7 @@
         <v>80</v>
       </c>
       <c r="L81" s="1">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -4257,7 +4259,7 @@
         <v>93</v>
       </c>
       <c r="L83" s="1">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -4333,7 +4335,7 @@
         <v>73</v>
       </c>
       <c r="L85" s="1">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add documentation to create_next_season_initial_roster function, replace 'team' with 'university' for consistency with other notebooks
</commit_message>
<xml_diff>
--- a/data/datasets/roster_fresno_state.xlsx
+++ b/data/datasets/roster_fresno_state.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B7C727-B99F-4029-9275-9B378C9F21EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="2029" sheetId="1" r:id="rId1"/>
     <sheet name="2030" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -719,11 +713,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+    <numFmt numFmtId="164" formatCode="#,##0;[Red]-#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,78 +758,62 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
+    <dxf/>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0;[Red]\-#,##0"/>
+      <numFmt numFmtId="164" formatCode="#,##0;[Red]-#,##0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:L85" totalsRowShown="0">
-  <autoFilter ref="A1:L85" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:L85" totalsRowShown="0">
+  <autoFilter ref="A1:L85"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="first_name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="last_name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="class"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="red_shirt"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="position"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="group"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="secondary_group"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="team"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="archetype"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="dev_trait"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="overall_start" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="overall_end" dataDxfId="2"/>
+    <tableColumn id="1" name="first_name" dataDxfId="0"/>
+    <tableColumn id="2" name="last_name" dataDxfId="0"/>
+    <tableColumn id="3" name="class" dataDxfId="0"/>
+    <tableColumn id="4" name="red_shirt" dataDxfId="0"/>
+    <tableColumn id="5" name="position" dataDxfId="0"/>
+    <tableColumn id="6" name="group" dataDxfId="0"/>
+    <tableColumn id="7" name="secondary_group" dataDxfId="0"/>
+    <tableColumn id="8" name="team" dataDxfId="0"/>
+    <tableColumn id="9" name="archetype" dataDxfId="0"/>
+    <tableColumn id="10" name="dev_trait" dataDxfId="0"/>
+    <tableColumn id="11" name="overall_start" dataDxfId="1"/>
+    <tableColumn id="12" name="overall_end" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Frame1" displayName="Frame1" ref="A1:L76" totalsRowShown="0">
-  <autoFilter ref="A1:L76" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Frame1" displayName="Frame1" ref="A1:L76" totalsRowShown="0">
+  <autoFilter ref="A1:L76"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="first_name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="last_name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="class"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="red_shirt"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="position"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="group"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="secondary_group"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="team"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="archetype"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="dev_trait"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="overall_start" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="overall_end" dataDxfId="0"/>
+    <tableColumn id="1" name="first_name" dataDxfId="0"/>
+    <tableColumn id="2" name="last_name" dataDxfId="0"/>
+    <tableColumn id="3" name="class" dataDxfId="0"/>
+    <tableColumn id="4" name="red_shirt" dataDxfId="0"/>
+    <tableColumn id="5" name="position" dataDxfId="0"/>
+    <tableColumn id="6" name="group" dataDxfId="0"/>
+    <tableColumn id="7" name="secondary_group" dataDxfId="0"/>
+    <tableColumn id="8" name="team" dataDxfId="0"/>
+    <tableColumn id="9" name="archetype" dataDxfId="0"/>
+    <tableColumn id="10" name="dev_trait" dataDxfId="0"/>
+    <tableColumn id="11" name="overall_start" dataDxfId="1"/>
+    <tableColumn id="12" name="overall_end" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -873,7 +851,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -907,7 +885,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -942,10 +919,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1118,14 +1094,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1201,7 +1177,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1239,7 +1215,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1277,7 +1253,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1315,7 +1291,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1353,7 +1329,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -1391,7 +1367,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1429,7 +1405,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -1467,7 +1443,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1505,7 +1481,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1543,7 +1519,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1581,7 +1557,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1619,7 +1595,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -1657,7 +1633,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1695,7 +1671,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1733,7 +1709,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -1771,7 +1747,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -1809,7 +1785,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>66</v>
       </c>
@@ -1847,7 +1823,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -1885,7 +1861,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
@@ -1923,7 +1899,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
@@ -1961,7 +1937,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>75</v>
       </c>
@@ -1999,7 +1975,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>79</v>
       </c>
@@ -2037,7 +2013,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2075,7 +2051,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -2113,7 +2089,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
@@ -2151,7 +2127,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
@@ -2189,7 +2165,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
@@ -2227,7 +2203,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>95</v>
       </c>
@@ -2265,7 +2241,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
@@ -2303,7 +2279,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>101</v>
       </c>
@@ -2341,7 +2317,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>103</v>
       </c>
@@ -2379,7 +2355,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>106</v>
       </c>
@@ -2417,7 +2393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>109</v>
       </c>
@@ -2455,7 +2431,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>111</v>
       </c>
@@ -2493,7 +2469,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
         <v>114</v>
       </c>
@@ -2531,7 +2507,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>116</v>
       </c>
@@ -2569,7 +2545,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>118</v>
       </c>
@@ -2607,7 +2583,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>121</v>
       </c>
@@ -2645,7 +2621,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>123</v>
       </c>
@@ -2683,7 +2659,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>125</v>
       </c>
@@ -2721,7 +2697,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -2759,7 +2735,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -2797,7 +2773,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
         <v>136</v>
       </c>
@@ -2835,7 +2811,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>138</v>
       </c>
@@ -2873,7 +2849,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>140</v>
       </c>
@@ -2911,7 +2887,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -2949,7 +2925,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
         <v>144</v>
       </c>
@@ -2987,7 +2963,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
         <v>146</v>
       </c>
@@ -3025,7 +3001,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
@@ -3063,7 +3039,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="A52" s="1" t="s">
         <v>150</v>
       </c>
@@ -3101,7 +3077,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
         <v>144</v>
       </c>
@@ -3139,7 +3115,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12">
       <c r="A54" s="1" t="s">
         <v>154</v>
       </c>
@@ -3177,7 +3153,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
@@ -3215,7 +3191,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12">
       <c r="A56" s="1" t="s">
         <v>160</v>
       </c>
@@ -3253,7 +3229,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
         <v>162</v>
       </c>
@@ -3291,7 +3267,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
         <v>164</v>
       </c>
@@ -3329,7 +3305,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
         <v>168</v>
       </c>
@@ -3367,7 +3343,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
         <v>170</v>
       </c>
@@ -3405,7 +3381,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
         <v>172</v>
       </c>
@@ -3443,7 +3419,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12">
       <c r="A62" s="1" t="s">
         <v>174</v>
       </c>
@@ -3481,7 +3457,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
@@ -3519,7 +3495,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
         <v>178</v>
       </c>
@@ -3557,7 +3533,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
         <v>180</v>
       </c>
@@ -3595,7 +3571,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
         <v>182</v>
       </c>
@@ -3633,7 +3609,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
         <v>62</v>
       </c>
@@ -3671,7 +3647,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
         <v>188</v>
       </c>
@@ -3709,7 +3685,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12">
       <c r="A69" s="1" t="s">
         <v>190</v>
       </c>
@@ -3747,7 +3723,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
         <v>193</v>
       </c>
@@ -3785,7 +3761,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12">
       <c r="A71" s="1" t="s">
         <v>196</v>
       </c>
@@ -3823,7 +3799,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
@@ -3861,7 +3837,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12">
       <c r="A73" s="1" t="s">
         <v>199</v>
       </c>
@@ -3899,7 +3875,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12">
       <c r="A74" s="1" t="s">
         <v>201</v>
       </c>
@@ -3937,7 +3913,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12">
       <c r="A75" s="1" t="s">
         <v>203</v>
       </c>
@@ -3975,7 +3951,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12">
       <c r="A76" s="1" t="s">
         <v>205</v>
       </c>
@@ -4013,7 +3989,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12">
       <c r="A77" s="1" t="s">
         <v>207</v>
       </c>
@@ -4051,7 +4027,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12">
       <c r="A78" s="1" t="s">
         <v>211</v>
       </c>
@@ -4089,7 +4065,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12">
       <c r="A79" s="1" t="s">
         <v>214</v>
       </c>
@@ -4127,7 +4103,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12">
       <c r="A80" s="1" t="s">
         <v>138</v>
       </c>
@@ -4165,7 +4141,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12">
       <c r="A81" s="1" t="s">
         <v>218</v>
       </c>
@@ -4203,7 +4179,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12">
       <c r="A82" s="1" t="s">
         <v>220</v>
       </c>
@@ -4241,7 +4217,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12">
       <c r="A83" s="1" t="s">
         <v>222</v>
       </c>
@@ -4279,7 +4255,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12">
       <c r="A84" s="1" t="s">
         <v>226</v>
       </c>
@@ -4317,7 +4293,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12">
       <c r="A85" s="1" t="s">
         <v>228</v>
       </c>
@@ -4364,14 +4340,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4409,7 +4385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -4443,7 +4419,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -4477,7 +4453,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -4511,7 +4487,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -4545,7 +4521,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -4579,7 +4555,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -4613,7 +4589,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -4647,7 +4623,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -4681,7 +4657,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -4715,7 +4691,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -4749,7 +4725,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -4783,7 +4759,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -4817,7 +4793,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -4851,7 +4827,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
@@ -4885,7 +4861,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
@@ -4919,7 +4895,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
@@ -4953,7 +4929,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -4987,7 +4963,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -5021,7 +4997,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -5055,7 +5031,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>82</v>
       </c>
@@ -5089,7 +5065,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
@@ -5123,7 +5099,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>91</v>
       </c>
@@ -5157,7 +5133,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>93</v>
       </c>
@@ -5191,7 +5167,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>95</v>
       </c>
@@ -5225,7 +5201,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
@@ -5259,7 +5235,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>101</v>
       </c>
@@ -5293,7 +5269,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>103</v>
       </c>
@@ -5327,7 +5303,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>106</v>
       </c>
@@ -5361,7 +5337,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>109</v>
       </c>
@@ -5395,7 +5371,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>111</v>
       </c>
@@ -5429,7 +5405,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>114</v>
       </c>
@@ -5463,7 +5439,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>116</v>
       </c>
@@ -5497,7 +5473,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
@@ -5531,7 +5507,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>121</v>
       </c>
@@ -5565,7 +5541,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>123</v>
       </c>
@@ -5599,7 +5575,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
         <v>125</v>
       </c>
@@ -5633,7 +5609,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>127</v>
       </c>
@@ -5667,7 +5643,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>62</v>
       </c>
@@ -5701,7 +5677,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>136</v>
       </c>
@@ -5735,7 +5711,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>138</v>
       </c>
@@ -5769,7 +5745,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>140</v>
       </c>
@@ -5803,7 +5779,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -5837,7 +5813,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
         <v>144</v>
       </c>
@@ -5871,7 +5847,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
         <v>146</v>
       </c>
@@ -5905,7 +5881,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
@@ -5939,7 +5915,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
@@ -5973,7 +5949,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
@@ -6007,7 +5983,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
         <v>154</v>
       </c>
@@ -6041,7 +6017,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
         <v>82</v>
       </c>
@@ -6075,7 +6051,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
         <v>160</v>
       </c>
@@ -6109,7 +6085,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="A52" s="1" t="s">
         <v>162</v>
       </c>
@@ -6143,7 +6119,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
         <v>164</v>
       </c>
@@ -6177,7 +6153,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12">
       <c r="A54" s="1" t="s">
         <v>168</v>
       </c>
@@ -6211,7 +6187,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
         <v>172</v>
       </c>
@@ -6245,7 +6221,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
@@ -6279,7 +6255,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
         <v>178</v>
       </c>
@@ -6313,7 +6289,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
         <v>180</v>
       </c>
@@ -6347,7 +6323,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
         <v>182</v>
       </c>
@@ -6381,7 +6357,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
@@ -6415,7 +6391,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
         <v>188</v>
       </c>
@@ -6449,7 +6425,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12">
       <c r="A62" s="1" t="s">
         <v>190</v>
       </c>
@@ -6483,7 +6459,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
         <v>193</v>
       </c>
@@ -6517,7 +6493,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
         <v>196</v>
       </c>
@@ -6551,7 +6527,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
         <v>82</v>
       </c>
@@ -6585,7 +6561,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
         <v>199</v>
       </c>
@@ -6619,7 +6595,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
         <v>201</v>
       </c>
@@ -6653,7 +6629,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
         <v>203</v>
       </c>
@@ -6687,7 +6663,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12">
       <c r="A69" s="1" t="s">
         <v>205</v>
       </c>
@@ -6721,7 +6697,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
         <v>211</v>
       </c>
@@ -6755,7 +6731,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12">
       <c r="A71" s="1" t="s">
         <v>214</v>
       </c>
@@ -6789,7 +6765,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
         <v>138</v>
       </c>
@@ -6823,7 +6799,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12">
       <c r="A73" s="1" t="s">
         <v>218</v>
       </c>
@@ -6857,7 +6833,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12">
       <c r="A74" s="1" t="s">
         <v>220</v>
       </c>
@@ -6891,7 +6867,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12">
       <c r="A75" s="1" t="s">
         <v>226</v>
       </c>
@@ -6925,7 +6901,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12">
       <c r="A76" s="1" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
Add overall_end values for fresno state 2030
</commit_message>
<xml_diff>
--- a/data/datasets/roster_fresno_state.xlsx
+++ b/data/datasets/roster_fresno_state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA0B8E4-89C1-4449-858C-6E299D6494FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28518B74-34FF-4925-88D2-3686D57B7214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2029" sheetId="1" r:id="rId1"/>
@@ -973,7 +973,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:L85" totalsRowShown="0">
-  <autoFilter ref="A1:L85" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A1:L85" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="QB"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="first_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="last_name"/>
@@ -1302,7 +1308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
@@ -1498,7 +1504,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1536,7 +1542,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -1574,7 +1580,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1612,7 +1618,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1764,7 +1770,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -1840,7 +1846,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1878,7 +1884,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1916,7 +1922,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -1992,7 +1998,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>66</v>
       </c>
@@ -2030,7 +2036,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -2068,7 +2074,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
@@ -2144,7 +2150,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>75</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>79</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2258,7 +2264,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -2296,7 +2302,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
@@ -2334,7 +2340,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
@@ -2410,7 +2416,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>95</v>
       </c>
@@ -2448,7 +2454,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
@@ -2486,7 +2492,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>101</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>103</v>
       </c>
@@ -2562,7 +2568,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>106</v>
       </c>
@@ -2600,7 +2606,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>109</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>111</v>
       </c>
@@ -2676,7 +2682,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>114</v>
       </c>
@@ -2714,7 +2720,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>116</v>
       </c>
@@ -2752,7 +2758,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>118</v>
       </c>
@@ -2790,7 +2796,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>121</v>
       </c>
@@ -2828,7 +2834,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>123</v>
       </c>
@@ -2866,7 +2872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>125</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -2942,7 +2948,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -2980,7 +2986,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>136</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>138</v>
       </c>
@@ -3056,7 +3062,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>140</v>
       </c>
@@ -3094,7 +3100,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>144</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>146</v>
       </c>
@@ -3208,7 +3214,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>150</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>144</v>
       </c>
@@ -3322,7 +3328,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>154</v>
       </c>
@@ -3360,7 +3366,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
@@ -3398,7 +3404,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>160</v>
       </c>
@@ -3436,7 +3442,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>162</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>164</v>
       </c>
@@ -3512,7 +3518,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>168</v>
       </c>
@@ -3550,7 +3556,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>170</v>
       </c>
@@ -3588,7 +3594,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>172</v>
       </c>
@@ -3626,7 +3632,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>174</v>
       </c>
@@ -3664,7 +3670,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
@@ -3702,7 +3708,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>178</v>
       </c>
@@ -3740,7 +3746,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>180</v>
       </c>
@@ -3778,7 +3784,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>182</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>62</v>
       </c>
@@ -3854,7 +3860,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>188</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>190</v>
       </c>
@@ -3930,7 +3936,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>193</v>
       </c>
@@ -3968,7 +3974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>196</v>
       </c>
@@ -4006,7 +4012,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
@@ -4044,7 +4050,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>199</v>
       </c>
@@ -4082,7 +4088,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>201</v>
       </c>
@@ -4120,7 +4126,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>203</v>
       </c>
@@ -4158,7 +4164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>205</v>
       </c>
@@ -4196,7 +4202,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>207</v>
       </c>
@@ -4234,7 +4240,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>211</v>
       </c>
@@ -4272,7 +4278,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>214</v>
       </c>
@@ -4310,7 +4316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>138</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>218</v>
       </c>
@@ -4386,7 +4392,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>220</v>
       </c>
@@ -4424,7 +4430,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>222</v>
       </c>
@@ -4462,7 +4468,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>226</v>
       </c>
@@ -4500,7 +4506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>228</v>
       </c>
@@ -4550,8 +4556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4642,7 +4648,9 @@
       <c r="K2" s="2">
         <v>94</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2">
+        <v>98</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -4678,7 +4686,9 @@
       <c r="K3" s="2">
         <v>86</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2">
+        <v>92</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -4714,7 +4724,9 @@
       <c r="K4" s="2">
         <v>78</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -4750,7 +4762,9 @@
       <c r="K5" s="2">
         <v>78</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -4786,7 +4800,9 @@
       <c r="K6" s="2">
         <v>95</v>
       </c>
-      <c r="L6" s="2"/>
+      <c r="L6" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -4822,7 +4838,9 @@
       <c r="K7" s="2">
         <v>86</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -4858,7 +4876,9 @@
       <c r="K8" s="2">
         <v>83</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -4894,7 +4914,9 @@
       <c r="K9" s="3">
         <v>75</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -4930,17 +4952,19 @@
       <c r="K10" s="3">
         <v>74</v>
       </c>
-      <c r="L10" s="3"/>
+      <c r="L10" s="3">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>1</v>
@@ -4958,25 +4982,27 @@
         <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K11" s="2">
-        <v>88</v>
-      </c>
-      <c r="L11" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="L11" s="2">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>1</v>
@@ -4994,15 +5020,17 @@
         <v>16</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K12" s="2">
-        <v>87</v>
-      </c>
-      <c r="L12" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="L12" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -5038,7 +5066,9 @@
       <c r="K13" s="2">
         <v>87</v>
       </c>
-      <c r="L13" s="2"/>
+      <c r="L13" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -5074,7 +5104,9 @@
       <c r="K14" s="2">
         <v>78</v>
       </c>
-      <c r="L14" s="2"/>
+      <c r="L14" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -5110,7 +5142,9 @@
       <c r="K15" s="2">
         <v>77</v>
       </c>
-      <c r="L15" s="2"/>
+      <c r="L15" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -5146,7 +5180,9 @@
       <c r="K16" s="2">
         <v>75</v>
       </c>
-      <c r="L16" s="2"/>
+      <c r="L16" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -5182,7 +5218,9 @@
       <c r="K17" s="2">
         <v>73</v>
       </c>
-      <c r="L17" s="2"/>
+      <c r="L17" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -5218,7 +5256,9 @@
       <c r="K18" s="3">
         <v>68</v>
       </c>
-      <c r="L18" s="3"/>
+      <c r="L18" s="3">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -5254,7 +5294,9 @@
       <c r="K19" s="3">
         <v>69</v>
       </c>
-      <c r="L19" s="3"/>
+      <c r="L19" s="3">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -5290,7 +5332,9 @@
       <c r="K20" s="3">
         <v>64</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3">
+        <v>64</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -5326,7 +5370,9 @@
       <c r="K21" s="2">
         <v>89</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2">
+        <v>94</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -5362,14 +5408,16 @@
       <c r="K22" s="2">
         <v>83</v>
       </c>
-      <c r="L22" s="2"/>
+      <c r="L22" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
@@ -5393,19 +5441,21 @@
         <v>78</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="K23" s="2">
-        <v>76</v>
-      </c>
-      <c r="L23" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="L23" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>201</v>
+        <v>246</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>25</v>
@@ -5429,12 +5479,14 @@
         <v>78</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="K24" s="2">
-        <v>75</v>
-      </c>
-      <c r="L24" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="L24" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -5470,17 +5522,19 @@
       <c r="K25" s="3">
         <v>74</v>
       </c>
-      <c r="L25" s="3"/>
+      <c r="L25" s="3">
+        <v>74</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="b">
         <v>1</v>
@@ -5498,25 +5552,27 @@
         <v>16</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="K26" s="2">
         <v>85</v>
       </c>
-      <c r="L26" s="2"/>
+      <c r="L26" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="b">
         <v>1</v>
@@ -5534,15 +5590,17 @@
         <v>16</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="K27" s="2">
         <v>85</v>
       </c>
-      <c r="L27" s="2"/>
+      <c r="L27" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -5578,7 +5636,9 @@
       <c r="K28" s="2">
         <v>76</v>
       </c>
-      <c r="L28" s="2"/>
+      <c r="L28" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -5614,7 +5674,9 @@
       <c r="K29" s="2">
         <v>75</v>
       </c>
-      <c r="L29" s="2"/>
+      <c r="L29" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -5650,7 +5712,9 @@
       <c r="K30" s="2">
         <v>91</v>
       </c>
-      <c r="L30" s="2"/>
+      <c r="L30" s="2">
+        <v>97</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -5686,7 +5750,9 @@
       <c r="K31" s="2">
         <v>87</v>
       </c>
-      <c r="L31" s="2"/>
+      <c r="L31" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -5722,7 +5788,9 @@
       <c r="K32" s="2">
         <v>84</v>
       </c>
-      <c r="L32" s="2"/>
+      <c r="L32" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -5758,7 +5826,9 @@
       <c r="K33" s="2">
         <v>75</v>
       </c>
-      <c r="L33" s="2"/>
+      <c r="L33" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -5794,17 +5864,19 @@
       <c r="K34" s="2">
         <v>75</v>
       </c>
-      <c r="L34" s="2"/>
+      <c r="L34" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D35" s="1" t="b">
         <v>1</v>
@@ -5822,25 +5894,27 @@
         <v>16</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="K35" s="2">
-        <v>90</v>
-      </c>
-      <c r="L35" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="L35" s="2">
+        <v>91</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D36" s="1" t="b">
         <v>1</v>
@@ -5858,15 +5932,17 @@
         <v>16</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="K36" s="2">
-        <v>88</v>
-      </c>
-      <c r="L36" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="L36" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -5902,7 +5978,9 @@
       <c r="K37" s="2">
         <v>73</v>
       </c>
-      <c r="L37" s="2"/>
+      <c r="L37" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -5938,7 +6016,9 @@
       <c r="K38" s="2">
         <v>95</v>
       </c>
-      <c r="L38" s="2"/>
+      <c r="L38" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -5974,7 +6054,9 @@
       <c r="K39" s="2">
         <v>86</v>
       </c>
-      <c r="L39" s="2"/>
+      <c r="L39" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -6010,7 +6092,9 @@
       <c r="K40" s="2">
         <v>78</v>
       </c>
-      <c r="L40" s="2"/>
+      <c r="L40" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -6046,7 +6130,9 @@
       <c r="K41" s="2">
         <v>72</v>
       </c>
-      <c r="L41" s="2"/>
+      <c r="L41" s="2">
+        <v>72</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -6082,7 +6168,9 @@
       <c r="K42" s="2">
         <v>85</v>
       </c>
-      <c r="L42" s="2"/>
+      <c r="L42" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -6118,7 +6206,9 @@
       <c r="K43" s="2">
         <v>82</v>
       </c>
-      <c r="L43" s="2"/>
+      <c r="L43" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -6154,7 +6244,9 @@
       <c r="K44" s="3">
         <v>76</v>
       </c>
-      <c r="L44" s="3"/>
+      <c r="L44" s="3">
+        <v>76</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -6190,7 +6282,9 @@
       <c r="K45" s="2">
         <v>92</v>
       </c>
-      <c r="L45" s="2"/>
+      <c r="L45" s="2">
+        <v>92</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -6226,7 +6320,9 @@
       <c r="K46" s="2">
         <v>79</v>
       </c>
-      <c r="L46" s="2"/>
+      <c r="L46" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -6262,7 +6358,9 @@
       <c r="K47" s="3">
         <v>78</v>
       </c>
-      <c r="L47" s="3"/>
+      <c r="L47" s="3">
+        <v>79</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -6298,7 +6396,9 @@
       <c r="K48" s="3">
         <v>75</v>
       </c>
-      <c r="L48" s="3"/>
+      <c r="L48" s="3">
+        <v>75</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
@@ -6334,7 +6434,9 @@
       <c r="K49" s="2">
         <v>91</v>
       </c>
-      <c r="L49" s="2"/>
+      <c r="L49" s="2">
+        <v>95</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
@@ -6370,17 +6472,19 @@
       <c r="K50" s="2">
         <v>89</v>
       </c>
-      <c r="L50" s="2"/>
+      <c r="L50" s="2">
+        <v>93</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D51" s="1" t="b">
         <v>1</v>
@@ -6401,22 +6505,24 @@
         <v>135</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="K51" s="2">
-        <v>83</v>
-      </c>
-      <c r="L51" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="L51" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D52" s="1" t="b">
         <v>1</v>
@@ -6437,12 +6543,14 @@
         <v>135</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="K52" s="2">
-        <v>82</v>
-      </c>
-      <c r="L52" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="L52" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -6478,17 +6586,19 @@
       <c r="K53" s="2">
         <v>73</v>
       </c>
-      <c r="L53" s="2"/>
+      <c r="L53" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D54" s="1" t="b">
         <v>1</v>
@@ -6506,25 +6616,27 @@
         <v>132</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K54" s="2">
-        <v>94</v>
-      </c>
-      <c r="L54" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="L54" s="2">
+        <v>96</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D55" s="1" t="b">
         <v>1</v>
@@ -6542,22 +6654,24 @@
         <v>132</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K55" s="2">
-        <v>92</v>
-      </c>
-      <c r="L55" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="L55" s="2">
+        <v>95</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B56" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
@@ -6578,22 +6692,24 @@
         <v>132</v>
       </c>
       <c r="I56" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J56" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="K56" s="2">
-        <v>74</v>
-      </c>
-      <c r="L56" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="L56" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B57" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
@@ -6622,14 +6738,16 @@
       <c r="K57" s="2">
         <v>74</v>
       </c>
-      <c r="L57" s="2"/>
+      <c r="L57" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B58" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
@@ -6650,15 +6768,17 @@
         <v>132</v>
       </c>
       <c r="I58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J58" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="K58" s="2">
-        <v>72</v>
-      </c>
-      <c r="L58" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="L58" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
@@ -6694,14 +6814,16 @@
       <c r="K59" s="2">
         <v>96</v>
       </c>
-      <c r="L59" s="2"/>
+      <c r="L59" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>25</v>
@@ -6730,14 +6852,16 @@
       <c r="K60" s="2">
         <v>79</v>
       </c>
-      <c r="L60" s="2"/>
+      <c r="L60" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>25</v>
@@ -6766,7 +6890,9 @@
       <c r="K61" s="2">
         <v>79</v>
       </c>
-      <c r="L61" s="2"/>
+      <c r="L61" s="2">
+        <v>82</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
@@ -6802,7 +6928,9 @@
       <c r="K62" s="2">
         <v>95</v>
       </c>
-      <c r="L62" s="2"/>
+      <c r="L62" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
@@ -6838,7 +6966,9 @@
       <c r="K63" s="2">
         <v>93</v>
       </c>
-      <c r="L63" s="2"/>
+      <c r="L63" s="2">
+        <v>93</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
@@ -6874,7 +7004,9 @@
       <c r="K64" s="2">
         <v>75</v>
       </c>
-      <c r="L64" s="2"/>
+      <c r="L64" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -6910,7 +7042,9 @@
       <c r="K65" s="2">
         <v>73</v>
       </c>
-      <c r="L65" s="2"/>
+      <c r="L65" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
@@ -6946,7 +7080,9 @@
       <c r="K66" s="2">
         <v>94</v>
       </c>
-      <c r="L66" s="2"/>
+      <c r="L66" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
@@ -6982,7 +7118,9 @@
       <c r="K67" s="2">
         <v>90</v>
       </c>
-      <c r="L67" s="2"/>
+      <c r="L67" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
@@ -7018,17 +7156,19 @@
       <c r="K68" s="2">
         <v>88</v>
       </c>
-      <c r="L68" s="2"/>
+      <c r="L68" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>62</v>
+        <v>190</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D69" s="1" t="b">
         <v>1</v>
@@ -7046,25 +7186,27 @@
         <v>132</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="K69" s="2">
-        <v>96</v>
-      </c>
-      <c r="L69" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="L69" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>190</v>
+        <v>62</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D70" s="1" t="b">
         <v>1</v>
@@ -7082,15 +7224,17 @@
         <v>132</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="K70" s="2">
-        <v>94</v>
-      </c>
-      <c r="L70" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="L70" s="2">
+        <v>99</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -7126,7 +7270,9 @@
       <c r="K71" s="2">
         <v>92</v>
       </c>
-      <c r="L71" s="2"/>
+      <c r="L71" s="2">
+        <v>97</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
@@ -7162,14 +7308,16 @@
       <c r="K72" s="2">
         <v>86</v>
       </c>
-      <c r="L72" s="2"/>
+      <c r="L72" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>25</v>
@@ -7196,16 +7344,18 @@
         <v>29</v>
       </c>
       <c r="K73" s="2">
-        <v>85</v>
-      </c>
-      <c r="L73" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L73" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>25</v>
@@ -7232,9 +7382,11 @@
         <v>29</v>
       </c>
       <c r="K74" s="2">
+        <v>85</v>
+      </c>
+      <c r="L74" s="2">
         <v>86</v>
       </c>
-      <c r="L74" s="2"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -7270,7 +7422,9 @@
       <c r="K75" s="2">
         <v>76</v>
       </c>
-      <c r="L75" s="2"/>
+      <c r="L75" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -7306,7 +7460,9 @@
       <c r="K76" s="2">
         <v>74</v>
       </c>
-      <c r="L76" s="2"/>
+      <c r="L76" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -7342,7 +7498,9 @@
       <c r="K77" s="2">
         <v>74</v>
       </c>
-      <c r="L77" s="2"/>
+      <c r="L77" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
@@ -7378,7 +7536,9 @@
       <c r="K78" s="2">
         <v>86</v>
       </c>
-      <c r="L78" s="2"/>
+      <c r="L78" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
@@ -7414,7 +7574,9 @@
       <c r="K79" s="2">
         <v>77</v>
       </c>
-      <c r="L79" s="2"/>
+      <c r="L79" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
@@ -7450,7 +7612,9 @@
       <c r="K80" s="2">
         <v>76</v>
       </c>
-      <c r="L80" s="2"/>
+      <c r="L80" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
@@ -7486,7 +7650,9 @@
       <c r="K81" s="3">
         <v>73</v>
       </c>
-      <c r="L81" s="3"/>
+      <c r="L81" s="3">
+        <v>73</v>
+      </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
@@ -7522,7 +7688,9 @@
       <c r="K82" s="2">
         <v>88</v>
       </c>
-      <c r="L82" s="2"/>
+      <c r="L82" s="2">
+        <v>93</v>
+      </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
@@ -7558,7 +7726,9 @@
       <c r="K83" s="2">
         <v>83</v>
       </c>
-      <c r="L83" s="2"/>
+      <c r="L83" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -7594,7 +7764,9 @@
       <c r="K84" s="2">
         <v>75</v>
       </c>
-      <c r="L84" s="2"/>
+      <c r="L84" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
@@ -7630,7 +7802,9 @@
       <c r="K85" s="2">
         <v>76</v>
       </c>
-      <c r="L85" s="2"/>
+      <c r="L85" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
@@ -7666,7 +7840,9 @@
       <c r="K86" s="2">
         <v>76</v>
       </c>
-      <c r="L86" s="2"/>
+      <c r="L86" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>

</xml_diff>